<commit_message>
Revert "회의 한 뒤"
This reverts commit 0010b3ce78d06d9a98169b07ba9315c998b3a032.
</commit_message>
<xml_diff>
--- a/능력치 관련 기획(알바, 교육).xlsx
+++ b/능력치 관련 기획(알바, 교육).xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EQ1\Documents\GitHub\KaraMaker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\GitHub\KaraMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="28035" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="28035" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="능력치(Status)" sheetId="1" r:id="rId1"/>
     <sheet name="아르바이트(Part Time)" sheetId="4" r:id="rId2"/>
     <sheet name="교육(Education)" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="157">
   <si>
     <t>능력치 종류/설명</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -468,6 +467,10 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>Black Factory</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>Shrine</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -645,18 +648,6 @@
   </si>
   <si>
     <t>번호</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">확률 </t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black Factory</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>수치상승 평균/10</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -767,7 +758,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -789,13 +780,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -896,6 +884,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -931,6 +936,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1109,16 +1131,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="9.75" customWidth="1"/>
     <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.4375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
@@ -1133,28 +1155,28 @@
     <col min="23" max="23" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.6">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A2" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>21</v>
@@ -1165,7 +1187,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -1173,20 +1195,20 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D3" s="6">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -1194,7 +1216,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1203,7 +1225,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -1211,7 +1233,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1220,7 +1242,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -1228,7 +1250,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1237,7 +1259,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -1245,7 +1267,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1254,7 +1276,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -1262,7 +1284,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1271,7 +1293,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -1279,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1288,7 +1310,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -1296,7 +1318,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1305,7 +1327,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -1313,7 +1335,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1322,7 +1344,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -1330,7 +1352,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1339,7 +1361,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -1347,7 +1369,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1356,7 +1378,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A14" s="6">
         <v>11</v>
       </c>
@@ -1364,7 +1386,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1373,7 +1395,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A15" s="6">
         <v>12</v>
       </c>
@@ -1381,7 +1403,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1390,7 +1412,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A16" s="6">
         <v>13</v>
       </c>
@@ -1398,7 +1420,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1407,7 +1429,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A17" s="6">
         <v>14</v>
       </c>
@@ -1415,7 +1437,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1424,7 +1446,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A18" s="6">
         <v>15</v>
       </c>
@@ -1432,7 +1454,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1441,7 +1463,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A19" s="6">
         <v>16</v>
       </c>
@@ -1449,7 +1471,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1458,7 +1480,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A20" s="6">
         <v>17</v>
       </c>
@@ -1466,7 +1488,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1475,7 +1497,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A21" s="6">
         <v>18</v>
       </c>
@@ -1483,7 +1505,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1492,7 +1514,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A22" s="6">
         <v>19</v>
       </c>
@@ -1500,7 +1522,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1509,7 +1531,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A23" s="6">
         <v>20</v>
       </c>
@@ -1517,7 +1539,7 @@
         <v>43</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1539,41 +1561,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="2" width="8.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.8125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A1" s="1"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>42</v>
@@ -1600,7 +1621,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -1629,7 +1650,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1656,7 +1677,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1664,7 +1685,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D5" s="6">
         <v>12</v>
@@ -1683,7 +1704,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1691,7 +1712,7 @@
         <v>30</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D6" s="6">
         <v>12</v>
@@ -1710,7 +1731,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1718,7 +1739,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D7" s="6">
         <v>12</v>
@@ -1737,7 +1758,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1745,7 +1766,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D8" s="6">
         <v>13</v>
@@ -1764,7 +1785,7 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1772,7 +1793,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D9" s="6">
         <v>13</v>
@@ -1791,7 +1812,7 @@
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1799,7 +1820,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D10" s="6">
         <v>13</v>
@@ -1818,7 +1839,7 @@
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1826,7 +1847,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D11" s="6">
         <v>13</v>
@@ -1845,7 +1866,7 @@
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1853,7 +1874,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D12" s="6">
         <v>13</v>
@@ -1872,7 +1893,7 @@
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1880,7 +1901,7 @@
         <v>34</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D13" s="6">
         <v>14</v>
@@ -1899,7 +1920,7 @@
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1907,7 +1928,7 @@
         <v>35</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D14" s="6">
         <v>15</v>
@@ -1926,7 +1947,7 @@
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1934,7 +1955,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D15" s="6">
         <v>15</v>
@@ -1953,7 +1974,7 @@
       </c>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1961,7 +1982,7 @@
         <v>24</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="D16" s="6">
         <v>18</v>
@@ -1979,14 +2000,6 @@
         <v>62</v>
       </c>
       <c r="I16" s="6"/>
-    </row>
-    <row r="19" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J19" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>158</v>
-      </c>
     </row>
   </sheetData>
   <sortState ref="B3:I16">
@@ -2004,41 +2017,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" customWidth="1"/>
     <col min="3" max="3" width="9.875" customWidth="1"/>
-    <col min="4" max="4" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1" s="1"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A2" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>80</v>
@@ -2046,13 +2059,13 @@
       <c r="E2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>86</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -2060,7 +2073,7 @@
         <v>104</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>97</v>
@@ -2074,7 +2087,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -2082,7 +2095,7 @@
         <v>78</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>99</v>
@@ -2096,7 +2109,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -2104,7 +2117,7 @@
         <v>74</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>95</v>
@@ -2118,7 +2131,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -2126,7 +2139,7 @@
         <v>73</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>102</v>
@@ -2140,7 +2153,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -2148,7 +2161,7 @@
         <v>72</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>100</v>
@@ -2162,7 +2175,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -2170,7 +2183,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>90</v>
@@ -2184,7 +2197,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -2192,7 +2205,7 @@
         <v>71</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>83</v>
@@ -2206,7 +2219,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -2214,7 +2227,7 @@
         <v>75</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>105</v>
@@ -2228,7 +2241,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -2236,7 +2249,7 @@
         <v>76</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>89</v>
@@ -2250,7 +2263,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -2258,7 +2271,7 @@
         <v>82</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>101</v>
@@ -2272,7 +2285,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -2280,7 +2293,7 @@
         <v>77</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>91</v>
@@ -2294,7 +2307,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2304,7 +2317,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2314,7 +2327,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2324,7 +2337,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2334,7 +2347,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2354,17 +2367,4 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "회의 한 뒤""
This reverts commit ccb5396629cdccb4ced51ba8264afd7911e49735.
</commit_message>
<xml_diff>
--- a/능력치 관련 기획(알바, 교육).xlsx
+++ b/능력치 관련 기획(알바, 교육).xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\GitHub\KaraMaker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EQ1\Documents\GitHub\KaraMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="28035" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="28035" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="능력치(Status)" sheetId="1" r:id="rId1"/>
     <sheet name="아르바이트(Part Time)" sheetId="4" r:id="rId2"/>
     <sheet name="교육(Education)" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="159">
   <si>
     <t>능력치 종류/설명</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -467,187 +468,195 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>Shrine</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bar</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delivery</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Housework</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parenting</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mine</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Salon</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hunter</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Graveyard</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tutor</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>영어이름</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magic</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fence</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Etiquette</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dance</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Music</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Science</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Theology</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Art</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Athletic</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Literature</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speech</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 아르바이트와 교육을 할 때마다 상승</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>영어 이름</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stress</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cleaning</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cook</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Talk</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elegance</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Courtesy</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Causation</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sensibility</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Health</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Strength</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intelligence</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Charisma</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Charm</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack Power</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spell</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Morality</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anti Spell</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Religiosity</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>번호</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">확률 </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>Black Factory</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Shrine</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bar</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Delivery</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Housework</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Parenting</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mine</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Salon</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hunter</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Graveyard</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tutor</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>영어이름</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Magic</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fence</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Etiquette</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dance</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Music</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Science</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Theology</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Art</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Athletic</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Literature</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speech</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>모든 아르바이트와 교육을 할 때마다 상승</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>영어 이름</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stress</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cleaning</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cook</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Talk</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Elegance</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Courtesy</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Causation</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sensibility</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Character</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Health</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Strength</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intelligence</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Charisma</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Charm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack Power</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Spell</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Morality</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Anti Spell</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Religiosity</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>번호</t>
+    <t>수치상승 평균/10</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -758,7 +767,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -780,10 +789,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -884,23 +896,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -936,23 +931,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1131,16 +1109,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.75" customWidth="1"/>
     <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.4375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
@@ -1155,28 +1133,28 @@
     <col min="23" max="23" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>21</v>
@@ -1187,7 +1165,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -1195,20 +1173,20 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D3" s="6">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -1216,7 +1194,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1225,7 +1203,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -1233,7 +1211,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1242,7 +1220,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -1250,7 +1228,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1259,7 +1237,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -1267,7 +1245,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1276,7 +1254,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -1284,7 +1262,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1293,7 +1271,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -1301,7 +1279,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1310,7 +1288,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -1318,7 +1296,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1327,7 +1305,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -1335,7 +1313,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1344,7 +1322,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -1352,7 +1330,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1361,7 +1339,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -1369,7 +1347,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1378,7 +1356,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>11</v>
       </c>
@@ -1386,7 +1364,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1395,7 +1373,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>12</v>
       </c>
@@ -1403,7 +1381,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1412,7 +1390,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>13</v>
       </c>
@@ -1420,7 +1398,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1429,7 +1407,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>14</v>
       </c>
@@ -1437,7 +1415,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1446,7 +1424,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>15</v>
       </c>
@@ -1454,7 +1432,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1463,7 +1441,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>16</v>
       </c>
@@ -1471,7 +1449,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1480,7 +1458,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>17</v>
       </c>
@@ -1488,7 +1466,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1497,7 +1475,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>18</v>
       </c>
@@ -1505,7 +1483,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1514,7 +1492,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>19</v>
       </c>
@@ -1522,7 +1500,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1531,7 +1509,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>20</v>
       </c>
@@ -1539,7 +1517,7 @@
         <v>43</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1561,40 +1539,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.8125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.6">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>42</v>
@@ -1621,7 +1600,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -1650,7 +1629,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1677,7 +1656,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1685,7 +1664,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" s="6">
         <v>12</v>
@@ -1704,7 +1683,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1712,7 +1691,7 @@
         <v>30</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" s="6">
         <v>12</v>
@@ -1731,7 +1710,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1739,7 +1718,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" s="6">
         <v>12</v>
@@ -1758,7 +1737,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1766,7 +1745,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" s="6">
         <v>13</v>
@@ -1785,7 +1764,7 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1793,7 +1772,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D9" s="6">
         <v>13</v>
@@ -1812,7 +1791,7 @@
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1820,7 +1799,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D10" s="6">
         <v>13</v>
@@ -1839,7 +1818,7 @@
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1847,7 +1826,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D11" s="6">
         <v>13</v>
@@ -1866,7 +1845,7 @@
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1874,7 +1853,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D12" s="6">
         <v>13</v>
@@ -1893,7 +1872,7 @@
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1901,7 +1880,7 @@
         <v>34</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D13" s="6">
         <v>14</v>
@@ -1920,7 +1899,7 @@
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1928,7 +1907,7 @@
         <v>35</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D14" s="6">
         <v>15</v>
@@ -1947,7 +1926,7 @@
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1955,7 +1934,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D15" s="6">
         <v>15</v>
@@ -1974,7 +1953,7 @@
       </c>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1982,7 +1961,7 @@
         <v>24</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
       <c r="D16" s="6">
         <v>18</v>
@@ -2000,6 +1979,14 @@
         <v>62</v>
       </c>
       <c r="I16" s="6"/>
+    </row>
+    <row r="19" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J19" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>158</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="B3:I16">
@@ -2017,41 +2004,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" customWidth="1"/>
     <col min="3" max="3" width="9.875" customWidth="1"/>
-    <col min="4" max="4" width="19.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>80</v>
@@ -2059,13 +2046,13 @@
       <c r="E2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>86</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -2073,7 +2060,7 @@
         <v>104</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>97</v>
@@ -2087,7 +2074,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -2095,7 +2082,7 @@
         <v>78</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>99</v>
@@ -2109,7 +2096,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -2117,7 +2104,7 @@
         <v>74</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>95</v>
@@ -2131,7 +2118,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -2139,7 +2126,7 @@
         <v>73</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>102</v>
@@ -2153,7 +2140,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -2161,7 +2148,7 @@
         <v>72</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>100</v>
@@ -2175,7 +2162,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -2183,7 +2170,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>90</v>
@@ -2197,7 +2184,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -2205,7 +2192,7 @@
         <v>71</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>83</v>
@@ -2219,7 +2206,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -2227,7 +2214,7 @@
         <v>75</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>105</v>
@@ -2241,7 +2228,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -2249,7 +2236,7 @@
         <v>76</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>89</v>
@@ -2263,7 +2250,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -2271,7 +2258,7 @@
         <v>82</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>101</v>
@@ -2285,7 +2272,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -2293,7 +2280,7 @@
         <v>77</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>91</v>
@@ -2307,7 +2294,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2317,7 +2304,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2327,7 +2314,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2337,7 +2324,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2347,7 +2334,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2367,4 +2354,17 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>